<commit_message>
Update TODO list and excersises
</commit_message>
<xml_diff>
--- a/Projekt_3_PDU.xlsx
+++ b/Projekt_3_PDU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDIA\MiNI PW\PDU\Prace projektowe\Projekt 3\Lioion-vikmf-gqhfcwrpse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{698DDDEC-D1DB-4B30-B715-41B9AA8B2F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E59BE31F-62EC-4C1F-B832-728CE1E24467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59FD8F85-3728-4529-BA16-F4594DCE6C27}"/>
   </bookViews>
@@ -175,12 +175,6 @@
     </r>
   </si>
   <si>
-    <t>16:15 - 18:00, 20:30 - ∞</t>
-  </si>
-  <si>
-    <t>Porównywanie zainteresowań po wieku użytkowników</t>
-  </si>
-  <si>
     <t>Ilość graczy zainteresowana w planszówkach i w grach komputerowych</t>
   </si>
   <si>
@@ -244,7 +238,13 @@
     <t>cenimy sobie gościnność</t>
   </si>
   <si>
-    <t>12:30 - 14:00, 19:00</t>
+    <t>16:15 - 18:00, 20:30 - 04:00</t>
+  </si>
+  <si>
+    <t>12:30 - 14:00, 19:00 - inf</t>
+  </si>
+  <si>
+    <t>Porównywanie zainteresowań po wieku użytkowników???</t>
   </si>
 </sst>
 </file>
@@ -334,13 +334,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,21 +440,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -463,6 +448,21 @@
       </right>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -663,9 +663,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -673,95 +673,57 @@
     <xf numFmtId="20" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -770,13 +732,47 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -806,7 +802,7 @@
     <xdr:ext cx="65" cy="172227"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="pole tekstowe 1">
+        <xdr:cNvPr id="3" name="pole tekstowe 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22037AD1-A278-AB47-90AD-220D921B39F6}"/>
@@ -1153,235 +1149,236 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33304EAE-8CE7-4A14-81C4-0C847C3794EF}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="86" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.109375" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.44140625" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="17" width="13.21875" customWidth="1"/>
+    <col min="17" max="17" width="13.109375" customWidth="1"/>
     <col min="18" max="18" width="11.44140625" customWidth="1"/>
     <col min="22" max="22" width="57.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
       <c r="E1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="35"/>
-      <c r="K2" s="25" t="s">
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="46"/>
+      <c r="K2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B3" s="44">
+        <v>44341</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="K3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B4" s="38"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="K4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="30">
-        <v>44341</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="K3" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="14"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="K4" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" s="48" t="s">
+      <c r="L4" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="18" t="s">
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="14"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="12" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="K5" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" s="50" t="s">
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="K5" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="51"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="14"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="12" t="s">
+      <c r="B6" s="38"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="K6" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="K6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="12" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="K7" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="18" t="s">
-        <v>33</v>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="K7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="13" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="K8" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="L8" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="45"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="48"/>
+      <c r="K8" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="14">
+      <c r="B9" s="38">
         <v>44343</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="C9" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
-      <c r="C10" s="16"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="40"/>
       <c r="D10" s="7" t="s">
         <v>12</v>
       </c>
@@ -1392,102 +1389,104 @@
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="14"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="11" t="s">
+      <c r="B11" s="38"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
     </row>
     <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="14"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="L12" s="37" t="s">
+      <c r="B12" s="38"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="L12" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="N12" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="M12" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="N12" s="36" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="L13" s="38" t="s">
+      <c r="B13" s="38"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="L13" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="L14" s="20" t="s">
+      <c r="B14" s="38"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="L14" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="9">
         <v>44344</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+        <v>52</v>
+      </c>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
       <c r="L15" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
+    <row r="16" spans="1:18" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="52">
+        <v>44345</v>
+      </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
       <c r="L16" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="L17" s="39" t="s">
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="L17" s="23" t="s">
         <v>18</v>
       </c>
       <c r="R17" s="8"/>
@@ -1496,100 +1495,104 @@
     <row r="18" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="L18" s="21" t="s">
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="L18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M18" s="40" t="s">
+      <c r="M18" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="N18" s="41" t="s">
+      <c r="N18" s="25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="L19" s="22" t="s">
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="L19" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
       <c r="L20" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
       <c r="L21" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="L22" s="20" t="s">
-        <v>33</v>
+      <c r="L22" s="13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="R24" s="43"/>
+      <c r="R24" s="26"/>
     </row>
     <row r="25" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L26" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="27"/>
-      <c r="Q26" s="28"/>
+      <c r="L26" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="32"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="L27" t="s">
+      <c r="L27" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="M27" s="51"/>
+      <c r="N27" s="51"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="L28" s="51" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="L28" t="s">
-        <v>44</v>
-      </c>
+      <c r="M28" s="51"/>
+      <c r="N28" s="51"/>
     </row>
     <row r="31" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L32" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="M32" s="27"/>
-      <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
-      <c r="Q32" s="28"/>
+      <c r="L32" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="31"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="32"/>
     </row>
     <row r="33" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L33" t="s">
@@ -1607,8 +1610,8 @@
       </c>
     </row>
     <row r="36" spans="12:12" x14ac:dyDescent="0.3">
-      <c r="L36" s="52" t="s">
-        <v>52</v>
+      <c r="L36" s="27" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1637,15 +1640,15 @@
     <mergeCell ref="D19:I19"/>
     <mergeCell ref="D9:I9"/>
     <mergeCell ref="D11:I11"/>
+    <mergeCell ref="L7:Q7"/>
+    <mergeCell ref="L8:Q8"/>
+    <mergeCell ref="L32:Q32"/>
+    <mergeCell ref="L26:Q26"/>
     <mergeCell ref="L2:Q2"/>
     <mergeCell ref="L3:Q3"/>
     <mergeCell ref="L5:Q5"/>
     <mergeCell ref="L4:Q4"/>
     <mergeCell ref="L6:Q6"/>
-    <mergeCell ref="L7:Q7"/>
-    <mergeCell ref="L8:Q8"/>
-    <mergeCell ref="L32:Q32"/>
-    <mergeCell ref="L26:Q26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1654,6 +1657,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E64AA5A784ECF34DB47262804B679200" ma:contentTypeVersion="10" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="66c22a824841797ef32c56931516ea7f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d4fbc36a-57e8-4887-83ab-179a59ead254" xmlns:ns4="8ca86435-1ed6-49e7-9af4-fc37d6f4e058" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63069fc28fd3b0a2644c402c470d7c62" ns3:_="" ns4:_="">
     <xsd:import namespace="d4fbc36a-57e8-4887-83ab-179a59ead254"/>
@@ -1856,22 +1874,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D28FE09-ADEC-486A-9CAA-A935B475E7FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8ca86435-1ed6-49e7-9af4-fc37d6f4e058"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d4fbc36a-57e8-4887-83ab-179a59ead254"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A722F9B2-E5F9-420F-AC01-B9D1687D92CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DEE151C-A54F-4C61-AB87-6E6E76EA91BD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1888,29 +1916,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D28FE09-ADEC-486A-9CAA-A935B475E7FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8ca86435-1ed6-49e7-9af4-fc37d6f4e058"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d4fbc36a-57e8-4887-83ab-179a59ead254"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A722F9B2-E5F9-420F-AC01-B9D1687D92CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update TODO, new RProjekt file, new Presentation - beamer
</commit_message>
<xml_diff>
--- a/Projekt_3_PDU.xlsx
+++ b/Projekt_3_PDU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\STUDIA\MiNI PW\PDU\Prace projektowe\Projekt 3\Lioion-vikmf-gqhfcwrpse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E59BE31F-62EC-4C1F-B832-728CE1E24467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD02BA91-9FD9-478E-9BDC-01F6FB21ABA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59FD8F85-3728-4529-BA16-F4594DCE6C27}"/>
   </bookViews>
@@ -657,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -702,18 +702,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -726,53 +767,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1150,7 +1144,7 @@
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1170,11 +1164,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="E1" t="s">
         <v>7</v>
       </c>
@@ -1186,199 +1180,199 @@
       <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="46"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="39"/>
       <c r="K2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="32"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="47"/>
       <c r="R2" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="44">
+      <c r="B3" s="34">
         <v>44341</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
       <c r="K3" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="34" t="s">
+      <c r="L3" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
       <c r="R3" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="38"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
       <c r="K4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="36" t="s">
+      <c r="L4" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
       <c r="R4" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="38"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="42" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
       <c r="K5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="36" t="s">
+      <c r="L5" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="38"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="42" t="s">
+      <c r="B6" s="35"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
       <c r="K6" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="42" t="s">
+      <c r="B7" s="35"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
       <c r="K7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="36" t="s">
+      <c r="L7" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="45"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="45"/>
       <c r="R7" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="48" t="s">
+      <c r="B8" s="35"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
       <c r="K8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="28" t="s">
+      <c r="L8" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="45"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="38">
+      <c r="B9" s="35">
         <v>44343</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="40"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="7" t="s">
         <v>12</v>
       </c>
@@ -1389,58 +1383,58 @@
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="38"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="41" t="s">
+      <c r="B11" s="35"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="38"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="L12" s="49" t="s">
+      <c r="B12" s="35"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="L12" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="M12" s="50" t="s">
+      <c r="M12" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="N12" s="50" t="s">
+      <c r="N12" s="29" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="38"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
       <c r="L13" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="38"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
       <c r="L14" s="13" t="s">
         <v>15</v>
       </c>
@@ -1452,27 +1446,27 @@
       <c r="C15" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
       <c r="L15" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="52">
+      <c r="B16" s="31">
         <v>44345</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
       <c r="L16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1480,12 +1474,12 @@
     <row r="17" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
       <c r="L17" s="23" t="s">
         <v>18</v>
       </c>
@@ -1495,12 +1489,12 @@
     <row r="18" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
       <c r="L18" s="14" t="s">
         <v>19</v>
       </c>
@@ -1514,12 +1508,12 @@
     <row r="19" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
       <c r="L19" s="15" t="s">
         <v>20</v>
       </c>
@@ -1527,12 +1521,12 @@
     <row r="20" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
       <c r="L20" s="3" t="s">
         <v>21</v>
       </c>
@@ -1540,12 +1534,12 @@
     <row r="21" spans="2:19" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="41"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
       <c r="L21" s="3" t="s">
         <v>22</v>
       </c>
@@ -1560,39 +1554,39 @@
     </row>
     <row r="25" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L26" s="30" t="s">
+      <c r="L26" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="31"/>
-      <c r="Q26" s="32"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="47"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="L27" s="51" t="s">
+      <c r="L27" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="M27" s="51"/>
-      <c r="N27" s="51"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="L28" s="51" t="s">
+      <c r="L28" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
     </row>
     <row r="31" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L32" s="30" t="s">
+      <c r="L32" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="M32" s="31"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="31"/>
-      <c r="Q32" s="32"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="38"/>
+      <c r="Q32" s="47"/>
     </row>
     <row r="33" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L33" t="s">
@@ -1616,6 +1610,29 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="L7:Q7"/>
+    <mergeCell ref="L8:Q8"/>
+    <mergeCell ref="L32:Q32"/>
+    <mergeCell ref="L26:Q26"/>
+    <mergeCell ref="L2:Q2"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="L5:Q5"/>
+    <mergeCell ref="L4:Q4"/>
+    <mergeCell ref="L6:Q6"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="D17:I17"/>
+    <mergeCell ref="D18:I18"/>
+    <mergeCell ref="D19:I19"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="D20:I20"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="D12:I12"/>
+    <mergeCell ref="D13:I13"/>
+    <mergeCell ref="D14:I14"/>
+    <mergeCell ref="D15:I15"/>
+    <mergeCell ref="D16:I16"/>
     <mergeCell ref="D6:I6"/>
     <mergeCell ref="D7:I7"/>
     <mergeCell ref="B1:D1"/>
@@ -1626,29 +1643,6 @@
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="D8:I8"/>
     <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D20:I20"/>
-    <mergeCell ref="D21:I21"/>
-    <mergeCell ref="D12:I12"/>
-    <mergeCell ref="D13:I13"/>
-    <mergeCell ref="D14:I14"/>
-    <mergeCell ref="D15:I15"/>
-    <mergeCell ref="D16:I16"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="D17:I17"/>
-    <mergeCell ref="D18:I18"/>
-    <mergeCell ref="D19:I19"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="L7:Q7"/>
-    <mergeCell ref="L8:Q8"/>
-    <mergeCell ref="L32:Q32"/>
-    <mergeCell ref="L26:Q26"/>
-    <mergeCell ref="L2:Q2"/>
-    <mergeCell ref="L3:Q3"/>
-    <mergeCell ref="L5:Q5"/>
-    <mergeCell ref="L4:Q4"/>
-    <mergeCell ref="L6:Q6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1657,18 +1651,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1875,6 +1869,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A722F9B2-E5F9-420F-AC01-B9D1687D92CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D28FE09-ADEC-486A-9CAA-A935B475E7FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1887,14 +1889,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="d4fbc36a-57e8-4887-83ab-179a59ead254"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A722F9B2-E5F9-420F-AC01-B9D1687D92CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>